<commit_message>
distribution scatter plot draft
</commit_message>
<xml_diff>
--- a/Metadata/result_default_numQuery.xlsx
+++ b/Metadata/result_default_numQuery.xlsx
@@ -504,13 +504,13 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>24.16</v>
+        <v>20.81</v>
       </c>
       <c r="G2" t="n">
-        <v>14</v>
+        <v>14.2</v>
       </c>
       <c r="H2" t="n">
-        <v>111</v>
+        <v>83.66666666666667</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -542,13 +542,13 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>55.07</v>
+        <v>54.79833333333332</v>
       </c>
       <c r="G3" t="n">
-        <v>8.5</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="H3" t="n">
-        <v>49</v>
+        <v>63.66666666666666</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -580,13 +580,13 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>59.48</v>
+        <v>58.04666666666667</v>
       </c>
       <c r="G4" t="n">
         <v>7</v>
       </c>
       <c r="H4" t="n">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>

</xml_diff>